<commit_message>
fix: tamplate laporan penjualan
</commit_message>
<xml_diff>
--- a/public/export_template/template_penjualan.xlsx
+++ b/public/export_template/template_penjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B308891-D49E-4A8D-B18A-FA989EB032C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C814398A-18E1-40AA-A3E4-8CA490BBC848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30840" yWindow="-1095" windowWidth="30960" windowHeight="17520" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,19 +65,19 @@
     <t>QTY</t>
   </si>
   <si>
+    <t>Diskon Nota</t>
+  </si>
+  <si>
+    <t>Bayar</t>
+  </si>
+  <si>
+    <t>Sisa</t>
+  </si>
+  <si>
     <t>Jumlah</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>Diskon Nota</t>
-  </si>
-  <si>
-    <t>Bayar</t>
-  </si>
-  <si>
-    <t>Sisa</t>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -136,7 +136,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +476,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +488,8 @@
     <col min="5" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -558,19 +561,19 @@
         <v>8</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update LaporanPenjualanExport and related views to include location and format currency (point 19)
</commit_message>
<xml_diff>
--- a/public/export_template/template_penjualan.xlsx
+++ b/public/export_template/template_penjualan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C814398A-18E1-40AA-A3E4-8CA490BBC848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97EB854-9DDB-44D5-B3AA-BD242E79EF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -130,13 +128,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -473,106 +471,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2042D607-C4CF-4B06-A3C3-62AF1890DECA}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L7" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: update LaporanPenjualanExport to include additional columns and correct total calculations (point 21)
</commit_message>
<xml_diff>
--- a/public/export_template/template_penjualan.xlsx
+++ b/public/export_template/template_penjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97EB854-9DDB-44D5-B3AA-BD242E79EF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A48F6F-9478-4291-9D75-204BAAA9B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>BDR HALL</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Nama Pelanggan</t>
   </si>
   <si>
-    <t>Kode Bbarang</t>
-  </si>
-  <si>
     <t>merek</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>No. Nota</t>
+  </si>
+  <si>
+    <t>Kd. barang</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -137,6 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,30 +475,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2042D607-C4CF-4B06-A3C3-62AF1890DECA}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -505,9 +508,9 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -519,12 +522,12 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -535,49 +538,53 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:L2"/>
-    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B1:M2"/>
+    <mergeCell ref="B3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: laporan penjualan exporrt pdf and excel header and detail (point 4)
</commit_message>
<xml_diff>
--- a/public/export_template/template_penjualan.xlsx
+++ b/public/export_template/template_penjualan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A48F6F-9478-4291-9D75-204BAAA9B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF1BDDC-B48A-4042-947B-B4D7EC1BAEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
@@ -134,13 +134,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,70 +478,74 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="M4" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">

</xml_diff>

<commit_message>
fix: update header laporan stok excel
</commit_message>
<xml_diff>
--- a/public/export_template/template_penjualan.xlsx
+++ b/public/export_template/template_penjualan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF1BDDC-B48A-4042-947B-B4D7EC1BAEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F151E1-FF18-417F-9C79-18CB82D46294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,12 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -478,7 +477,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M1:M1048576"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,53 +498,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">

</xml_diff>